<commit_message>
adapted script to new template
</commit_message>
<xml_diff>
--- a/data/HAB_CostaRica.xlsx
+++ b/data/HAB_CostaRica.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="1533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="1532">
   <si>
     <t>HAB region</t>
   </si>
@@ -4394,9 +4394,6 @@
     <t>Verbatim depth</t>
   </si>
   <si>
-    <t>measurementUnits</t>
-  </si>
-  <si>
     <t>Other measurements</t>
   </si>
   <si>
@@ -4505,9 +4502,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>units</t>
-  </si>
-  <si>
     <t>Salinity</t>
   </si>
   <si>
@@ -4632,6 +4626,9 @@
   </si>
   <si>
     <t>the bloom had reached its broadest spatial extent of approximately 50km2, many fish species dead</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -5124,10 +5121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CL189"/>
+  <dimension ref="A1:CL163"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5240,7 +5237,7 @@
     </row>
     <row r="2" spans="1:90" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>0</v>
@@ -5249,7 +5246,7 @@
         <v>1067</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>1068</v>
@@ -5282,10 +5279,10 @@
         <v>1112</v>
       </c>
       <c r="S2" s="8" t="s">
+        <v>1469</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>1470</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>1471</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>1107</v>
@@ -5294,13 +5291,13 @@
         <v>1108</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>1114</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>1074</v>
@@ -5396,16 +5393,16 @@
         <v>1451</v>
       </c>
       <c r="BH2" s="8" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="BI2" s="8" t="s">
         <v>1099</v>
       </c>
       <c r="BJ2" s="8" t="s">
+        <v>1482</v>
+      </c>
+      <c r="BK2" s="8" t="s">
         <v>1483</v>
-      </c>
-      <c r="BK2" s="8" t="s">
-        <v>1484</v>
       </c>
       <c r="BL2" s="8" t="s">
         <v>1404</v>
@@ -5414,22 +5411,22 @@
         <v>1100</v>
       </c>
       <c r="BN2" s="8" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="BO2" s="8" t="s">
         <v>1101</v>
       </c>
       <c r="BP2" s="8" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="BQ2" s="8" t="s">
+        <v>1474</v>
+      </c>
+      <c r="BR2" s="8" t="s">
+        <v>1473</v>
+      </c>
+      <c r="BS2" s="8" t="s">
         <v>1475</v>
-      </c>
-      <c r="BR2" s="8" t="s">
-        <v>1474</v>
-      </c>
-      <c r="BS2" s="8" t="s">
-        <v>1476</v>
       </c>
       <c r="BT2" s="8" t="s">
         <v>1102</v>
@@ -5441,28 +5438,28 @@
         <v>1452</v>
       </c>
       <c r="BW2" s="8" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="BX2" s="8" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="BY2" s="8" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="CA2" s="8" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="CC2" s="10" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="CG2" s="8" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="CK2" s="8" t="s">
         <v>1110</v>
       </c>
       <c r="CL2" s="8" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="3" spans="1:90" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5502,40 +5499,40 @@
         <v>1445</v>
       </c>
       <c r="BY3" s="8" t="s">
+        <v>1487</v>
+      </c>
+      <c r="BZ3" s="8" t="s">
         <v>1488</v>
       </c>
-      <c r="BZ3" s="8" t="s">
-        <v>1489</v>
-      </c>
       <c r="CA3" s="10" t="s">
+        <v>1487</v>
+      </c>
+      <c r="CB3" s="10" t="s">
         <v>1488</v>
       </c>
-      <c r="CB3" s="10" t="s">
-        <v>1489</v>
-      </c>
       <c r="CC3" s="10" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="CD3" s="10" t="s">
+        <v>1487</v>
+      </c>
+      <c r="CE3" s="10" t="s">
+        <v>1531</v>
+      </c>
+      <c r="CF3" s="10" t="s">
         <v>1488</v>
       </c>
-      <c r="CE3" s="10" t="s">
-        <v>1490</v>
-      </c>
-      <c r="CF3" s="10" t="s">
-        <v>1489</v>
-      </c>
       <c r="CG3" s="10" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="CH3" s="10" t="s">
+        <v>1487</v>
+      </c>
+      <c r="CI3" s="10" t="s">
+        <v>1531</v>
+      </c>
+      <c r="CJ3" s="10" t="s">
         <v>1488</v>
-      </c>
-      <c r="CI3" s="10" t="s">
-        <v>1490</v>
-      </c>
-      <c r="CJ3" s="10" t="s">
-        <v>1489</v>
       </c>
     </row>
     <row r="4" spans="1:90" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -5786,7 +5783,7 @@
         <v>1423</v>
       </c>
       <c r="CE4" s="21" t="s">
-        <v>1453</v>
+        <v>1424</v>
       </c>
       <c r="CF4" s="21" t="s">
         <v>1422</v>
@@ -5798,7 +5795,7 @@
         <v>1423</v>
       </c>
       <c r="CI4" s="21" t="s">
-        <v>1453</v>
+        <v>1424</v>
       </c>
       <c r="CJ4" s="21" t="s">
         <v>1422</v>
@@ -5818,49 +5815,49 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D5" s="15">
         <v>42304</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>1495</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="J5" s="17" t="s">
         <v>1496</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="K5" s="17" t="s">
         <v>1497</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>1498</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>1499</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>1014</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="AA5" s="13" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="AG5" s="13" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="AH5" s="13" t="s">
         <v>1082</v>
       </c>
       <c r="AI5" s="13" t="s">
+        <v>1500</v>
+      </c>
+      <c r="AJ5" s="13" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AW5" s="18" t="s">
         <v>1502</v>
-      </c>
-      <c r="AJ5" s="13" t="s">
-        <v>1503</v>
-      </c>
-      <c r="AW5" s="18" t="s">
-        <v>1504</v>
       </c>
       <c r="AX5" s="18"/>
       <c r="AY5" s="18"/>
@@ -5871,19 +5868,19 @@
         <v>-84.65</v>
       </c>
       <c r="BG5" s="13" t="s">
+        <v>1503</v>
+      </c>
+      <c r="BH5" s="13" t="s">
+        <v>1504</v>
+      </c>
+      <c r="BI5" s="13" t="s">
         <v>1505</v>
       </c>
-      <c r="BH5" s="13" t="s">
+      <c r="BK5" s="13" t="s">
         <v>1506</v>
       </c>
-      <c r="BI5" s="13" t="s">
+      <c r="BN5" s="13" t="s">
         <v>1507</v>
-      </c>
-      <c r="BK5" s="13" t="s">
-        <v>1508</v>
-      </c>
-      <c r="BN5" s="13" t="s">
-        <v>1509</v>
       </c>
     </row>
     <row r="6" spans="1:90" x14ac:dyDescent="0.2">
@@ -5894,46 +5891,46 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D6" s="15">
         <v>42304</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>1508</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>1510</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="J6" s="17" t="s">
         <v>1511</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="K6" s="17" t="s">
         <v>1512</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>1513</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>1514</v>
       </c>
       <c r="P6" s="13" t="s">
         <v>1014</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="AA6" s="13" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="AH6" s="13" t="s">
         <v>1082</v>
       </c>
       <c r="AI6" s="13" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="AJ6" s="13" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="AW6" s="18"/>
       <c r="AX6" s="18"/>
@@ -5945,16 +5942,16 @@
         <v>-85.71</v>
       </c>
       <c r="BG6" s="13" t="s">
+        <v>1513</v>
+      </c>
+      <c r="BH6" s="13" t="s">
+        <v>1504</v>
+      </c>
+      <c r="BI6" s="13" t="s">
+        <v>1514</v>
+      </c>
+      <c r="BN6" s="13" t="s">
         <v>1515</v>
-      </c>
-      <c r="BH6" s="13" t="s">
-        <v>1506</v>
-      </c>
-      <c r="BI6" s="13" t="s">
-        <v>1516</v>
-      </c>
-      <c r="BN6" s="13" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="7" spans="1:90" x14ac:dyDescent="0.2">
@@ -5965,25 +5962,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D7" s="15">
         <v>42306</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>1516</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>1518</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="J7" s="17" t="s">
         <v>1519</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="K7" s="17" t="s">
         <v>1520</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>1521</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>1522</v>
       </c>
       <c r="P7" s="13" t="s">
         <v>303</v>
@@ -5992,54 +5989,54 @@
         <v>380000000</v>
       </c>
       <c r="R7" s="13" t="s">
+        <v>1521</v>
+      </c>
+      <c r="S7" s="13">
+        <v>1</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>1522</v>
+      </c>
+      <c r="U7" s="13" t="s">
         <v>1523</v>
       </c>
-      <c r="S7" s="13">
-        <v>1</v>
-      </c>
-      <c r="T7" s="13" t="s">
+      <c r="Y7" s="13" t="s">
+        <v>1530</v>
+      </c>
+      <c r="Z7" s="13" t="s">
+        <v>1464</v>
+      </c>
+      <c r="AA7" s="13" t="s">
         <v>1524</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="AB7" s="13" t="s">
+        <v>1467</v>
+      </c>
+      <c r="AC7" s="13" t="s">
+        <v>1464</v>
+      </c>
+      <c r="AD7" s="13" t="s">
         <v>1525</v>
       </c>
-      <c r="Y7" s="13" t="s">
-        <v>1532</v>
-      </c>
-      <c r="Z7" s="13" t="s">
-        <v>1465</v>
-      </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AE7" s="13" t="s">
         <v>1526</v>
       </c>
-      <c r="AB7" s="13" t="s">
-        <v>1468</v>
-      </c>
-      <c r="AC7" s="13" t="s">
-        <v>1465</v>
-      </c>
-      <c r="AD7" s="13" t="s">
+      <c r="AH7" s="13" t="s">
         <v>1527</v>
       </c>
-      <c r="AE7" s="13" t="s">
+      <c r="AN7" s="13" t="s">
         <v>1528</v>
       </c>
-      <c r="AH7" s="13" t="s">
-        <v>1529</v>
-      </c>
-      <c r="AN7" s="13" t="s">
-        <v>1530</v>
-      </c>
       <c r="AR7" s="13" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="AS7" s="13" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="AW7" s="18"/>
       <c r="AX7" s="18"/>
       <c r="AY7" s="18" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="AZ7" s="13">
         <v>9.9654000000000007</v>
@@ -6048,10 +6045,10 @@
         <v>-84.87</v>
       </c>
       <c r="BG7" s="13" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="BH7" s="13" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="8" spans="1:90" x14ac:dyDescent="0.2">
@@ -6071,6 +6068,7 @@
       <c r="AX10" s="18"/>
       <c r="AY10" s="18"/>
       <c r="AZ10" s="18"/>
+      <c r="BA10" s="18"/>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D11" s="15"/>
@@ -7096,206 +7094,24 @@
     </row>
     <row r="157" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D157" s="15"/>
-      <c r="AX157" s="18"/>
-      <c r="AY157" s="18"/>
-      <c r="AZ157" s="18"/>
-      <c r="BA157" s="18"/>
     </row>
     <row r="158" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D158" s="15"/>
-      <c r="AX158" s="18"/>
-      <c r="AY158" s="18"/>
-      <c r="AZ158" s="18"/>
-      <c r="BA158" s="18"/>
     </row>
     <row r="159" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D159" s="15"/>
-      <c r="AX159" s="18"/>
-      <c r="AY159" s="18"/>
-      <c r="AZ159" s="18"/>
-      <c r="BA159" s="18"/>
     </row>
     <row r="160" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D160" s="15"/>
-      <c r="AX160" s="18"/>
-      <c r="AY160" s="18"/>
-      <c r="AZ160" s="18"/>
-      <c r="BA160" s="18"/>
-    </row>
-    <row r="161" spans="4:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D161" s="15"/>
-      <c r="AX161" s="18"/>
-      <c r="AY161" s="18"/>
-      <c r="AZ161" s="18"/>
-      <c r="BA161" s="18"/>
-    </row>
-    <row r="162" spans="4:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D162" s="15"/>
-      <c r="AX162" s="18"/>
-      <c r="AY162" s="18"/>
-      <c r="AZ162" s="18"/>
-      <c r="BA162" s="18"/>
-    </row>
-    <row r="163" spans="4:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D163" s="15"/>
-      <c r="AX163" s="18"/>
-      <c r="AY163" s="18"/>
-      <c r="AZ163" s="18"/>
-      <c r="BA163" s="18"/>
-    </row>
-    <row r="164" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D164" s="15"/>
-      <c r="AX164" s="18"/>
-      <c r="AY164" s="18"/>
-      <c r="AZ164" s="18"/>
-      <c r="BA164" s="18"/>
-    </row>
-    <row r="165" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D165" s="15"/>
-      <c r="AX165" s="18"/>
-      <c r="AY165" s="18"/>
-      <c r="AZ165" s="18"/>
-      <c r="BA165" s="18"/>
-    </row>
-    <row r="166" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D166" s="15"/>
-      <c r="AX166" s="18"/>
-      <c r="AY166" s="18"/>
-      <c r="AZ166" s="18"/>
-      <c r="BA166" s="18"/>
-    </row>
-    <row r="167" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D167" s="15"/>
-      <c r="AX167" s="18"/>
-      <c r="AY167" s="18"/>
-      <c r="AZ167" s="18"/>
-      <c r="BA167" s="18"/>
-    </row>
-    <row r="168" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D168" s="15"/>
-      <c r="AX168" s="18"/>
-      <c r="AY168" s="18"/>
-      <c r="AZ168" s="18"/>
-      <c r="BA168" s="18"/>
-    </row>
-    <row r="169" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D169" s="15"/>
-      <c r="AX169" s="18"/>
-      <c r="AY169" s="18"/>
-      <c r="AZ169" s="18"/>
-      <c r="BA169" s="18"/>
-    </row>
-    <row r="170" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D170" s="15"/>
-      <c r="AX170" s="18"/>
-      <c r="AY170" s="18"/>
-      <c r="AZ170" s="18"/>
-      <c r="BA170" s="18"/>
-    </row>
-    <row r="171" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D171" s="15"/>
-      <c r="AX171" s="18"/>
-      <c r="AY171" s="18"/>
-      <c r="AZ171" s="18"/>
-      <c r="BA171" s="18"/>
-    </row>
-    <row r="172" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D172" s="15"/>
-      <c r="AX172" s="18"/>
-      <c r="AY172" s="18"/>
-      <c r="AZ172" s="18"/>
-      <c r="BA172" s="18"/>
-    </row>
-    <row r="173" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D173" s="15"/>
-      <c r="AX173" s="18"/>
-      <c r="AY173" s="18"/>
-      <c r="AZ173" s="18"/>
-      <c r="BA173" s="18"/>
-    </row>
-    <row r="174" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D174" s="15"/>
-      <c r="AX174" s="18"/>
-      <c r="AY174" s="18"/>
-      <c r="AZ174" s="18"/>
-      <c r="BA174" s="18"/>
-    </row>
-    <row r="175" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D175" s="15"/>
-      <c r="AX175" s="18"/>
-      <c r="AY175" s="18"/>
-      <c r="AZ175" s="18"/>
-      <c r="BA175" s="18"/>
-    </row>
-    <row r="176" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D176" s="15"/>
-      <c r="AX176" s="18"/>
-      <c r="AY176" s="18"/>
-      <c r="AZ176" s="18"/>
-      <c r="BA176" s="18"/>
-    </row>
-    <row r="177" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D177" s="15"/>
-      <c r="AX177" s="18"/>
-      <c r="AY177" s="18"/>
-      <c r="AZ177" s="18"/>
-      <c r="BA177" s="18"/>
-    </row>
-    <row r="178" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D178" s="15"/>
-      <c r="AX178" s="18"/>
-      <c r="AY178" s="18"/>
-      <c r="AZ178" s="18"/>
-      <c r="BA178" s="18"/>
-    </row>
-    <row r="179" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D179" s="15"/>
-      <c r="AX179" s="18"/>
-      <c r="AY179" s="18"/>
-      <c r="AZ179" s="18"/>
-      <c r="BA179" s="18"/>
-    </row>
-    <row r="180" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D180" s="15"/>
-      <c r="AX180" s="18"/>
-      <c r="AY180" s="18"/>
-      <c r="AZ180" s="18"/>
-      <c r="BA180" s="18"/>
-    </row>
-    <row r="181" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D181" s="15"/>
-      <c r="AX181" s="18"/>
-      <c r="AY181" s="18"/>
-      <c r="AZ181" s="18"/>
-      <c r="BA181" s="18"/>
-    </row>
-    <row r="182" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D182" s="15"/>
-      <c r="AX182" s="18"/>
-      <c r="AY182" s="18"/>
-      <c r="AZ182" s="18"/>
-      <c r="BA182" s="18"/>
-    </row>
-    <row r="183" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D183" s="15"/>
-    </row>
-    <row r="184" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D184" s="15"/>
-    </row>
-    <row r="185" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D185" s="15"/>
-    </row>
-    <row r="186" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D186" s="15"/>
-    </row>
-    <row r="187" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D187" s="15"/>
-    </row>
-    <row r="188" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D188" s="15"/>
-    </row>
-    <row r="189" spans="4:53" x14ac:dyDescent="0.2">
-      <c r="D189" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7305,51 +7121,51 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>syndromes!$A$1:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG5:AG7 AH8:AH1242</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>lists!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>BQ5:BQ7 BR8:BR1082</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>lists!$D$1:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>BV5:BV7 BW8:BW1243</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>regions!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B1297</xm:sqref>
+          <xm:sqref>B5:B1271</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Z5:Z1217</xm:sqref>
+          <xm:sqref>Z5:Z1191</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>AB5:AB1159</xm:sqref>
+          <xm:sqref>AB5:AB1133</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>AF5:AF1184</xm:sqref>
+          <xm:sqref>AF5:AF1158</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>toxins!$A$2:$A$246</xm:f>
           </x14:formula1>
-          <xm:sqref>AG8:AG1236</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>syndromes!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>AH8:AH1268 AG5:AG7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>lists!$C$1:$C$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>BR8:BR1108 BQ5:BQ7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>lists!$D$1:$D$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>BW8:BW1269 BV5:BV7</xm:sqref>
+          <xm:sqref>AG8:AG1210</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7373,10 +7189,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1456</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1457</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -33511,10 +33327,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1461</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1462</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -33535,10 +33351,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -33559,7 +33375,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1383</v>
@@ -33642,43 +33458,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B1" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="C1" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="D1" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B2" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="C2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="D2" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D3" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>